<commit_message>
Update bug-report for M3
</commit_message>
<xml_diff>
--- a/doc/bug-report.xlsx
+++ b/doc/bug-report.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="664" uniqueCount="356">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="698" uniqueCount="364">
   <si>
     <t>CPSC 427 - Bug List for Seekers (Team 23)</t>
   </si>
@@ -1132,9 +1132,6 @@
     <t>#163</t>
   </si>
   <si>
-    <t>In-Progress</t>
-  </si>
-  <si>
     <t>Improvement: Entity collision push back feels unnatural</t>
   </si>
   <si>
@@ -1168,6 +1165,9 @@
   </si>
   <si>
     <t>#166</t>
+  </si>
+  <si>
+    <t>In-Progress</t>
   </si>
   <si>
     <t>Bug: Enemies can pass through walls during push back interactions</t>
@@ -1266,6 +1266,55 @@
   </si>
   <si>
     <t>Planned for Milestone 3</t>
+  </si>
+  <si>
+    <t>Feat: Save at bonfire</t>
+  </si>
+  <si>
+    <t>Save should happen automatically at bonfire</t>
+  </si>
+  <si>
+    <t>Save through keyboard keys</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+        <sz val="11.0"/>
+      </rPr>
+      <t xml:space="preserve">Related Issues: </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color rgb="FF1155CC"/>
+        <sz val="11.0"/>
+        <u/>
+      </rPr>
+      <t>#163</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+        <sz val="11.0"/>
+      </rPr>
+      <t xml:space="preserve"> (Entity Collision Push Back)</t>
+    </r>
+  </si>
+  <si>
+    <t>Bug: Zombie AI attack you before you are within attack range</t>
+  </si>
+  <si>
+    <t>Zombie AI attack should attack only within attack range</t>
+  </si>
+  <si>
+    <t>Zombie AI attack you before you are within attack range</t>
+  </si>
+  <si>
+    <t>1. Walk close to zombie AI but from distance
+2. Zombie will attack outside range</t>
   </si>
   <si>
     <t>Severity</t>
@@ -1729,6 +1778,9 @@
     <xf borderId="8" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
+    <xf borderId="5" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
     <xf borderId="9" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
@@ -1737,9 +1789,6 @@
     </xf>
     <xf borderId="9" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="6" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
@@ -5023,10 +5072,10 @@
         <v>216</v>
       </c>
       <c r="D62" s="15" t="s">
-        <v>268</v>
+        <v>154</v>
       </c>
       <c r="E62" s="16" t="s">
-        <v>269</v>
+        <v>14</v>
       </c>
       <c r="F62" s="14" t="s">
         <v>282</v>
@@ -5355,23 +5404,23 @@
         <v>59</v>
       </c>
       <c r="E69" s="25" t="s">
-        <v>317</v>
+        <v>14</v>
       </c>
       <c r="F69" s="23" t="s">
         <v>282</v>
       </c>
       <c r="G69" s="27" t="s">
+        <v>317</v>
+      </c>
+      <c r="H69" s="27" t="s">
         <v>318</v>
       </c>
-      <c r="H69" s="27" t="s">
+      <c r="I69" s="27" t="s">
         <v>319</v>
-      </c>
-      <c r="I69" s="27" t="s">
-        <v>320</v>
       </c>
       <c r="J69" s="27"/>
       <c r="K69" s="42" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="L69" s="20"/>
       <c r="M69" s="20"/>
@@ -5391,7 +5440,7 @@
     </row>
     <row r="70" ht="14.25" customHeight="1">
       <c r="A70" s="38" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B70" s="30">
         <v>45598.0</v>
@@ -5409,16 +5458,16 @@
         <v>282</v>
       </c>
       <c r="G70" s="18" t="s">
+        <v>322</v>
+      </c>
+      <c r="H70" s="18" t="s">
         <v>323</v>
       </c>
-      <c r="H70" s="18" t="s">
+      <c r="I70" s="18" t="s">
         <v>324</v>
       </c>
-      <c r="I70" s="18" t="s">
+      <c r="J70" s="18" t="s">
         <v>325</v>
-      </c>
-      <c r="J70" s="18" t="s">
-        <v>326</v>
       </c>
       <c r="K70" s="46"/>
       <c r="L70" s="20"/>
@@ -5439,7 +5488,7 @@
     </row>
     <row r="71" ht="14.25" customHeight="1">
       <c r="A71" s="40" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B71" s="34">
         <v>45598.0</v>
@@ -5451,7 +5500,7 @@
         <v>59</v>
       </c>
       <c r="E71" s="25" t="s">
-        <v>269</v>
+        <v>327</v>
       </c>
       <c r="F71" s="23" t="s">
         <v>41</v>
@@ -5633,14 +5682,30 @@
     </row>
     <row r="75" ht="14.25" customHeight="1">
       <c r="A75" s="48"/>
-      <c r="B75" s="49"/>
-      <c r="C75" s="50"/>
-      <c r="D75" s="51"/>
-      <c r="E75" s="25"/>
-      <c r="F75" s="23"/>
-      <c r="G75" s="27"/>
-      <c r="H75" s="27"/>
-      <c r="I75" s="27"/>
+      <c r="B75" s="22">
+        <v>45615.0</v>
+      </c>
+      <c r="C75" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="D75" s="24" t="s">
+        <v>154</v>
+      </c>
+      <c r="E75" s="25" t="s">
+        <v>269</v>
+      </c>
+      <c r="F75" s="23" t="s">
+        <v>282</v>
+      </c>
+      <c r="G75" s="27" t="s">
+        <v>348</v>
+      </c>
+      <c r="H75" s="27" t="s">
+        <v>349</v>
+      </c>
+      <c r="I75" s="27" t="s">
+        <v>350</v>
+      </c>
       <c r="J75" s="27"/>
       <c r="K75" s="42"/>
       <c r="L75" s="20"/>
@@ -5660,16 +5725,36 @@
       <c r="Z75" s="20"/>
     </row>
     <row r="76" ht="14.25" customHeight="1">
-      <c r="A76" s="52"/>
-      <c r="B76" s="53"/>
-      <c r="C76" s="54"/>
-      <c r="D76" s="55"/>
-      <c r="E76" s="16"/>
-      <c r="F76" s="14"/>
-      <c r="G76" s="18"/>
-      <c r="H76" s="18"/>
-      <c r="I76" s="18"/>
-      <c r="J76" s="18"/>
+      <c r="A76" s="38" t="s">
+        <v>321</v>
+      </c>
+      <c r="B76" s="30">
+        <v>45612.0</v>
+      </c>
+      <c r="C76" s="14" t="s">
+        <v>216</v>
+      </c>
+      <c r="D76" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="E76" s="16" t="s">
+        <v>269</v>
+      </c>
+      <c r="F76" s="14" t="s">
+        <v>282</v>
+      </c>
+      <c r="G76" s="18" t="s">
+        <v>322</v>
+      </c>
+      <c r="H76" s="18" t="s">
+        <v>323</v>
+      </c>
+      <c r="I76" s="18" t="s">
+        <v>324</v>
+      </c>
+      <c r="J76" s="18" t="s">
+        <v>325</v>
+      </c>
       <c r="K76" s="46"/>
       <c r="L76" s="20"/>
       <c r="M76" s="20"/>
@@ -5688,17 +5773,39 @@
       <c r="Z76" s="20"/>
     </row>
     <row r="77" ht="14.25" customHeight="1">
-      <c r="A77" s="48"/>
-      <c r="B77" s="49"/>
-      <c r="C77" s="50"/>
-      <c r="D77" s="51"/>
-      <c r="E77" s="25"/>
-      <c r="F77" s="23"/>
-      <c r="G77" s="27"/>
-      <c r="H77" s="27"/>
-      <c r="I77" s="27"/>
-      <c r="J77" s="27"/>
-      <c r="K77" s="42"/>
+      <c r="A77" s="40" t="s">
+        <v>326</v>
+      </c>
+      <c r="B77" s="34">
+        <v>45612.0</v>
+      </c>
+      <c r="C77" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="D77" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="E77" s="25" t="s">
+        <v>327</v>
+      </c>
+      <c r="F77" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="G77" s="27" t="s">
+        <v>328</v>
+      </c>
+      <c r="H77" s="27" t="s">
+        <v>329</v>
+      </c>
+      <c r="I77" s="27" t="s">
+        <v>330</v>
+      </c>
+      <c r="J77" s="27" t="s">
+        <v>331</v>
+      </c>
+      <c r="K77" s="47" t="s">
+        <v>351</v>
+      </c>
       <c r="L77" s="20"/>
       <c r="M77" s="20"/>
       <c r="N77" s="20"/>
@@ -5716,16 +5823,34 @@
       <c r="Z77" s="20"/>
     </row>
     <row r="78" ht="14.25" customHeight="1">
-      <c r="A78" s="52"/>
-      <c r="B78" s="53"/>
-      <c r="C78" s="54"/>
-      <c r="D78" s="55"/>
-      <c r="E78" s="16"/>
-      <c r="F78" s="14"/>
-      <c r="G78" s="18"/>
-      <c r="H78" s="18"/>
-      <c r="I78" s="18"/>
-      <c r="J78" s="18"/>
+      <c r="A78" s="49"/>
+      <c r="B78" s="13">
+        <v>45612.0</v>
+      </c>
+      <c r="C78" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="D78" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="E78" s="16" t="s">
+        <v>269</v>
+      </c>
+      <c r="F78" s="14" t="s">
+        <v>282</v>
+      </c>
+      <c r="G78" s="18" t="s">
+        <v>352</v>
+      </c>
+      <c r="H78" s="18" t="s">
+        <v>353</v>
+      </c>
+      <c r="I78" s="18" t="s">
+        <v>354</v>
+      </c>
+      <c r="J78" s="18" t="s">
+        <v>355</v>
+      </c>
       <c r="K78" s="46"/>
       <c r="L78" s="20"/>
       <c r="M78" s="20"/>
@@ -5745,9 +5870,9 @@
     </row>
     <row r="79" ht="14.25" customHeight="1">
       <c r="A79" s="48"/>
-      <c r="B79" s="49"/>
-      <c r="C79" s="50"/>
-      <c r="D79" s="51"/>
+      <c r="B79" s="50"/>
+      <c r="C79" s="51"/>
+      <c r="D79" s="52"/>
       <c r="E79" s="25"/>
       <c r="F79" s="23"/>
       <c r="G79" s="27"/>
@@ -5772,7 +5897,7 @@
       <c r="Z79" s="20"/>
     </row>
     <row r="80" ht="14.25" customHeight="1">
-      <c r="A80" s="52"/>
+      <c r="A80" s="49"/>
       <c r="B80" s="53"/>
       <c r="C80" s="54"/>
       <c r="D80" s="55"/>
@@ -5801,9 +5926,9 @@
     </row>
     <row r="81" ht="14.25" customHeight="1">
       <c r="A81" s="48"/>
-      <c r="B81" s="49"/>
-      <c r="C81" s="50"/>
-      <c r="D81" s="51"/>
+      <c r="B81" s="50"/>
+      <c r="C81" s="51"/>
+      <c r="D81" s="52"/>
       <c r="E81" s="25"/>
       <c r="F81" s="23"/>
       <c r="G81" s="27"/>
@@ -5828,7 +5953,7 @@
       <c r="Z81" s="20"/>
     </row>
     <row r="82" ht="14.25" customHeight="1">
-      <c r="A82" s="52"/>
+      <c r="A82" s="49"/>
       <c r="B82" s="53"/>
       <c r="C82" s="54"/>
       <c r="D82" s="55"/>
@@ -5857,9 +5982,9 @@
     </row>
     <row r="83" ht="14.25" customHeight="1">
       <c r="A83" s="48"/>
-      <c r="B83" s="49"/>
-      <c r="C83" s="50"/>
-      <c r="D83" s="51"/>
+      <c r="B83" s="50"/>
+      <c r="C83" s="51"/>
+      <c r="D83" s="52"/>
       <c r="E83" s="25"/>
       <c r="F83" s="23"/>
       <c r="G83" s="27"/>
@@ -5884,7 +6009,7 @@
       <c r="Z83" s="20"/>
     </row>
     <row r="84" ht="14.25" customHeight="1">
-      <c r="A84" s="52"/>
+      <c r="A84" s="49"/>
       <c r="B84" s="53"/>
       <c r="C84" s="54"/>
       <c r="D84" s="55"/>
@@ -5913,9 +6038,9 @@
     </row>
     <row r="85" ht="14.25" customHeight="1">
       <c r="A85" s="48"/>
-      <c r="B85" s="49"/>
-      <c r="C85" s="50"/>
-      <c r="D85" s="51"/>
+      <c r="B85" s="50"/>
+      <c r="C85" s="51"/>
+      <c r="D85" s="52"/>
       <c r="E85" s="25"/>
       <c r="F85" s="23"/>
       <c r="G85" s="27"/>
@@ -5940,7 +6065,7 @@
       <c r="Z85" s="20"/>
     </row>
     <row r="86" ht="14.25" customHeight="1">
-      <c r="A86" s="52"/>
+      <c r="A86" s="49"/>
       <c r="B86" s="53"/>
       <c r="C86" s="54"/>
       <c r="D86" s="55"/>
@@ -5969,9 +6094,9 @@
     </row>
     <row r="87" ht="14.25" customHeight="1">
       <c r="A87" s="48"/>
-      <c r="B87" s="49"/>
-      <c r="C87" s="50"/>
-      <c r="D87" s="51"/>
+      <c r="B87" s="50"/>
+      <c r="C87" s="51"/>
+      <c r="D87" s="52"/>
       <c r="E87" s="25"/>
       <c r="F87" s="23"/>
       <c r="G87" s="27"/>
@@ -5996,7 +6121,7 @@
       <c r="Z87" s="20"/>
     </row>
     <row r="88" ht="14.25" customHeight="1">
-      <c r="A88" s="52"/>
+      <c r="A88" s="49"/>
       <c r="B88" s="53"/>
       <c r="C88" s="54"/>
       <c r="D88" s="55"/>
@@ -6025,9 +6150,9 @@
     </row>
     <row r="89" ht="14.25" customHeight="1">
       <c r="A89" s="48"/>
-      <c r="B89" s="49"/>
-      <c r="C89" s="50"/>
-      <c r="D89" s="51"/>
+      <c r="B89" s="50"/>
+      <c r="C89" s="51"/>
+      <c r="D89" s="52"/>
       <c r="E89" s="25"/>
       <c r="F89" s="23"/>
       <c r="G89" s="27"/>
@@ -6052,7 +6177,7 @@
       <c r="Z89" s="20"/>
     </row>
     <row r="90" ht="14.25" customHeight="1">
-      <c r="A90" s="52"/>
+      <c r="A90" s="49"/>
       <c r="B90" s="53"/>
       <c r="C90" s="54"/>
       <c r="D90" s="55"/>
@@ -6081,9 +6206,9 @@
     </row>
     <row r="91" ht="14.25" customHeight="1">
       <c r="A91" s="48"/>
-      <c r="B91" s="49"/>
-      <c r="C91" s="50"/>
-      <c r="D91" s="51"/>
+      <c r="B91" s="50"/>
+      <c r="C91" s="51"/>
+      <c r="D91" s="52"/>
       <c r="E91" s="25"/>
       <c r="F91" s="23"/>
       <c r="G91" s="27"/>
@@ -6108,7 +6233,7 @@
       <c r="Z91" s="20"/>
     </row>
     <row r="92" ht="14.25" customHeight="1">
-      <c r="A92" s="52"/>
+      <c r="A92" s="49"/>
       <c r="B92" s="53"/>
       <c r="C92" s="54"/>
       <c r="D92" s="55"/>
@@ -6137,9 +6262,9 @@
     </row>
     <row r="93" ht="14.25" customHeight="1">
       <c r="A93" s="48"/>
-      <c r="B93" s="49"/>
-      <c r="C93" s="50"/>
-      <c r="D93" s="51"/>
+      <c r="B93" s="50"/>
+      <c r="C93" s="51"/>
+      <c r="D93" s="52"/>
       <c r="E93" s="25"/>
       <c r="F93" s="23"/>
       <c r="G93" s="27"/>
@@ -6164,7 +6289,7 @@
       <c r="Z93" s="20"/>
     </row>
     <row r="94" ht="14.25" customHeight="1">
-      <c r="A94" s="52"/>
+      <c r="A94" s="49"/>
       <c r="B94" s="53"/>
       <c r="C94" s="54"/>
       <c r="D94" s="55"/>
@@ -6193,9 +6318,9 @@
     </row>
     <row r="95" ht="14.25" customHeight="1">
       <c r="A95" s="48"/>
-      <c r="B95" s="49"/>
-      <c r="C95" s="50"/>
-      <c r="D95" s="51"/>
+      <c r="B95" s="50"/>
+      <c r="C95" s="51"/>
+      <c r="D95" s="52"/>
       <c r="E95" s="25"/>
       <c r="F95" s="23"/>
       <c r="G95" s="27"/>
@@ -6220,7 +6345,7 @@
       <c r="Z95" s="20"/>
     </row>
     <row r="96" ht="14.25" customHeight="1">
-      <c r="A96" s="52"/>
+      <c r="A96" s="49"/>
       <c r="B96" s="53"/>
       <c r="C96" s="54"/>
       <c r="D96" s="55"/>
@@ -6249,9 +6374,9 @@
     </row>
     <row r="97" ht="14.25" customHeight="1">
       <c r="A97" s="48"/>
-      <c r="B97" s="49"/>
-      <c r="C97" s="50"/>
-      <c r="D97" s="51"/>
+      <c r="B97" s="50"/>
+      <c r="C97" s="51"/>
+      <c r="D97" s="52"/>
       <c r="E97" s="25"/>
       <c r="F97" s="23"/>
       <c r="G97" s="27"/>
@@ -6276,7 +6401,7 @@
       <c r="Z97" s="20"/>
     </row>
     <row r="98" ht="14.25" customHeight="1">
-      <c r="A98" s="52"/>
+      <c r="A98" s="49"/>
       <c r="B98" s="53"/>
       <c r="C98" s="54"/>
       <c r="D98" s="55"/>
@@ -6305,9 +6430,9 @@
     </row>
     <row r="99" ht="14.25" customHeight="1">
       <c r="A99" s="48"/>
-      <c r="B99" s="49"/>
-      <c r="C99" s="50"/>
-      <c r="D99" s="51"/>
+      <c r="B99" s="50"/>
+      <c r="C99" s="51"/>
+      <c r="D99" s="52"/>
       <c r="E99" s="25"/>
       <c r="F99" s="23"/>
       <c r="G99" s="27"/>
@@ -6332,7 +6457,7 @@
       <c r="Z99" s="20"/>
     </row>
     <row r="100" ht="14.25" customHeight="1">
-      <c r="A100" s="52"/>
+      <c r="A100" s="49"/>
       <c r="B100" s="53"/>
       <c r="C100" s="54"/>
       <c r="D100" s="55"/>
@@ -6361,9 +6486,9 @@
     </row>
     <row r="101" ht="14.25" customHeight="1">
       <c r="A101" s="48"/>
-      <c r="B101" s="49"/>
-      <c r="C101" s="50"/>
-      <c r="D101" s="51"/>
+      <c r="B101" s="50"/>
+      <c r="C101" s="51"/>
+      <c r="D101" s="52"/>
       <c r="E101" s="25"/>
       <c r="F101" s="23"/>
       <c r="G101" s="27"/>
@@ -6388,7 +6513,7 @@
       <c r="Z101" s="20"/>
     </row>
     <row r="102" ht="14.25" customHeight="1">
-      <c r="A102" s="52"/>
+      <c r="A102" s="49"/>
       <c r="B102" s="53"/>
       <c r="C102" s="54"/>
       <c r="D102" s="55"/>
@@ -6417,9 +6542,9 @@
     </row>
     <row r="103" ht="14.25" customHeight="1">
       <c r="A103" s="48"/>
-      <c r="B103" s="49"/>
-      <c r="C103" s="50"/>
-      <c r="D103" s="51"/>
+      <c r="B103" s="50"/>
+      <c r="C103" s="51"/>
+      <c r="D103" s="52"/>
       <c r="E103" s="25"/>
       <c r="F103" s="23"/>
       <c r="G103" s="27"/>
@@ -6444,7 +6569,7 @@
       <c r="Z103" s="20"/>
     </row>
     <row r="104" ht="14.25" customHeight="1">
-      <c r="A104" s="52"/>
+      <c r="A104" s="49"/>
       <c r="B104" s="53"/>
       <c r="C104" s="54"/>
       <c r="D104" s="55"/>
@@ -6473,9 +6598,9 @@
     </row>
     <row r="105" ht="14.25" customHeight="1">
       <c r="A105" s="48"/>
-      <c r="B105" s="49"/>
-      <c r="C105" s="50"/>
-      <c r="D105" s="51"/>
+      <c r="B105" s="50"/>
+      <c r="C105" s="51"/>
+      <c r="D105" s="52"/>
       <c r="E105" s="25"/>
       <c r="F105" s="23"/>
       <c r="G105" s="27"/>
@@ -6500,7 +6625,7 @@
       <c r="Z105" s="20"/>
     </row>
     <row r="106" ht="14.25" customHeight="1">
-      <c r="A106" s="52"/>
+      <c r="A106" s="49"/>
       <c r="B106" s="53"/>
       <c r="C106" s="54"/>
       <c r="D106" s="55"/>
@@ -6529,9 +6654,9 @@
     </row>
     <row r="107" ht="14.25" customHeight="1">
       <c r="A107" s="48"/>
-      <c r="B107" s="49"/>
-      <c r="C107" s="50"/>
-      <c r="D107" s="51"/>
+      <c r="B107" s="50"/>
+      <c r="C107" s="51"/>
+      <c r="D107" s="52"/>
       <c r="E107" s="25"/>
       <c r="F107" s="23"/>
       <c r="G107" s="27"/>
@@ -6556,7 +6681,7 @@
       <c r="Z107" s="20"/>
     </row>
     <row r="108" ht="14.25" customHeight="1">
-      <c r="A108" s="52"/>
+      <c r="A108" s="49"/>
       <c r="B108" s="53"/>
       <c r="C108" s="54"/>
       <c r="D108" s="55"/>
@@ -6585,9 +6710,9 @@
     </row>
     <row r="109" ht="14.25" customHeight="1">
       <c r="A109" s="48"/>
-      <c r="B109" s="49"/>
-      <c r="C109" s="50"/>
-      <c r="D109" s="51"/>
+      <c r="B109" s="50"/>
+      <c r="C109" s="51"/>
+      <c r="D109" s="52"/>
       <c r="E109" s="25"/>
       <c r="F109" s="23"/>
       <c r="G109" s="27"/>
@@ -6612,7 +6737,7 @@
       <c r="Z109" s="20"/>
     </row>
     <row r="110" ht="14.25" customHeight="1">
-      <c r="A110" s="52"/>
+      <c r="A110" s="49"/>
       <c r="B110" s="53"/>
       <c r="C110" s="54"/>
       <c r="D110" s="55"/>
@@ -6641,9 +6766,9 @@
     </row>
     <row r="111" ht="14.25" customHeight="1">
       <c r="A111" s="48"/>
-      <c r="B111" s="49"/>
-      <c r="C111" s="50"/>
-      <c r="D111" s="51"/>
+      <c r="B111" s="50"/>
+      <c r="C111" s="51"/>
+      <c r="D111" s="52"/>
       <c r="E111" s="25"/>
       <c r="F111" s="23"/>
       <c r="G111" s="27"/>
@@ -6668,7 +6793,7 @@
       <c r="Z111" s="20"/>
     </row>
     <row r="112" ht="14.25" customHeight="1">
-      <c r="A112" s="52"/>
+      <c r="A112" s="49"/>
       <c r="B112" s="53"/>
       <c r="C112" s="54"/>
       <c r="D112" s="55"/>
@@ -6697,9 +6822,9 @@
     </row>
     <row r="113" ht="14.25" customHeight="1">
       <c r="A113" s="48"/>
-      <c r="B113" s="49"/>
-      <c r="C113" s="50"/>
-      <c r="D113" s="51"/>
+      <c r="B113" s="50"/>
+      <c r="C113" s="51"/>
+      <c r="D113" s="52"/>
       <c r="E113" s="25"/>
       <c r="F113" s="23"/>
       <c r="G113" s="27"/>
@@ -6724,7 +6849,7 @@
       <c r="Z113" s="20"/>
     </row>
     <row r="114" ht="14.25" customHeight="1">
-      <c r="A114" s="52"/>
+      <c r="A114" s="49"/>
       <c r="B114" s="53"/>
       <c r="C114" s="54"/>
       <c r="D114" s="55"/>
@@ -6753,9 +6878,9 @@
     </row>
     <row r="115" ht="14.25" customHeight="1">
       <c r="A115" s="48"/>
-      <c r="B115" s="49"/>
-      <c r="C115" s="50"/>
-      <c r="D115" s="51"/>
+      <c r="B115" s="50"/>
+      <c r="C115" s="51"/>
+      <c r="D115" s="52"/>
       <c r="E115" s="25"/>
       <c r="F115" s="23"/>
       <c r="G115" s="27"/>
@@ -6780,7 +6905,7 @@
       <c r="Z115" s="20"/>
     </row>
     <row r="116" ht="14.25" customHeight="1">
-      <c r="A116" s="52"/>
+      <c r="A116" s="49"/>
       <c r="B116" s="53"/>
       <c r="C116" s="54"/>
       <c r="D116" s="55"/>
@@ -6809,9 +6934,9 @@
     </row>
     <row r="117" ht="14.25" customHeight="1">
       <c r="A117" s="48"/>
-      <c r="B117" s="49"/>
-      <c r="C117" s="50"/>
-      <c r="D117" s="51"/>
+      <c r="B117" s="50"/>
+      <c r="C117" s="51"/>
+      <c r="D117" s="52"/>
       <c r="E117" s="25"/>
       <c r="F117" s="23"/>
       <c r="G117" s="27"/>
@@ -6836,7 +6961,7 @@
       <c r="Z117" s="20"/>
     </row>
     <row r="118" ht="14.25" customHeight="1">
-      <c r="A118" s="52"/>
+      <c r="A118" s="49"/>
       <c r="B118" s="53"/>
       <c r="C118" s="54"/>
       <c r="D118" s="55"/>
@@ -6865,9 +6990,9 @@
     </row>
     <row r="119" ht="14.25" customHeight="1">
       <c r="A119" s="48"/>
-      <c r="B119" s="49"/>
-      <c r="C119" s="50"/>
-      <c r="D119" s="51"/>
+      <c r="B119" s="50"/>
+      <c r="C119" s="51"/>
+      <c r="D119" s="52"/>
       <c r="E119" s="25"/>
       <c r="F119" s="23"/>
       <c r="G119" s="27"/>
@@ -6892,7 +7017,7 @@
       <c r="Z119" s="20"/>
     </row>
     <row r="120" ht="14.25" customHeight="1">
-      <c r="A120" s="52"/>
+      <c r="A120" s="49"/>
       <c r="B120" s="53"/>
       <c r="C120" s="54"/>
       <c r="D120" s="55"/>
@@ -6921,9 +7046,9 @@
     </row>
     <row r="121" ht="14.25" customHeight="1">
       <c r="A121" s="48"/>
-      <c r="B121" s="49"/>
-      <c r="C121" s="50"/>
-      <c r="D121" s="51"/>
+      <c r="B121" s="50"/>
+      <c r="C121" s="51"/>
+      <c r="D121" s="52"/>
       <c r="E121" s="25"/>
       <c r="F121" s="23"/>
       <c r="G121" s="27"/>
@@ -6948,7 +7073,7 @@
       <c r="Z121" s="20"/>
     </row>
     <row r="122" ht="14.25" customHeight="1">
-      <c r="A122" s="52"/>
+      <c r="A122" s="49"/>
       <c r="B122" s="53"/>
       <c r="C122" s="54"/>
       <c r="D122" s="55"/>
@@ -6977,9 +7102,9 @@
     </row>
     <row r="123" ht="14.25" customHeight="1">
       <c r="A123" s="48"/>
-      <c r="B123" s="49"/>
-      <c r="C123" s="50"/>
-      <c r="D123" s="51"/>
+      <c r="B123" s="50"/>
+      <c r="C123" s="51"/>
+      <c r="D123" s="52"/>
       <c r="E123" s="25"/>
       <c r="F123" s="23"/>
       <c r="G123" s="27"/>
@@ -7004,7 +7129,7 @@
       <c r="Z123" s="20"/>
     </row>
     <row r="124" ht="14.25" customHeight="1">
-      <c r="A124" s="52"/>
+      <c r="A124" s="49"/>
       <c r="B124" s="53"/>
       <c r="C124" s="54"/>
       <c r="D124" s="55"/>
@@ -7033,9 +7158,9 @@
     </row>
     <row r="125" ht="14.25" customHeight="1">
       <c r="A125" s="48"/>
-      <c r="B125" s="49"/>
-      <c r="C125" s="50"/>
-      <c r="D125" s="51"/>
+      <c r="B125" s="50"/>
+      <c r="C125" s="51"/>
+      <c r="D125" s="52"/>
       <c r="E125" s="25"/>
       <c r="F125" s="23"/>
       <c r="G125" s="27"/>
@@ -7060,7 +7185,7 @@
       <c r="Z125" s="20"/>
     </row>
     <row r="126" ht="14.25" customHeight="1">
-      <c r="A126" s="52"/>
+      <c r="A126" s="49"/>
       <c r="B126" s="53"/>
       <c r="C126" s="54"/>
       <c r="D126" s="55"/>
@@ -7089,9 +7214,9 @@
     </row>
     <row r="127" ht="14.25" customHeight="1">
       <c r="A127" s="48"/>
-      <c r="B127" s="49"/>
-      <c r="C127" s="50"/>
-      <c r="D127" s="51"/>
+      <c r="B127" s="50"/>
+      <c r="C127" s="51"/>
+      <c r="D127" s="52"/>
       <c r="E127" s="25"/>
       <c r="F127" s="23"/>
       <c r="G127" s="27"/>
@@ -7116,7 +7241,7 @@
       <c r="Z127" s="20"/>
     </row>
     <row r="128" ht="14.25" customHeight="1">
-      <c r="A128" s="52"/>
+      <c r="A128" s="49"/>
       <c r="B128" s="53"/>
       <c r="C128" s="54"/>
       <c r="D128" s="55"/>
@@ -7145,9 +7270,9 @@
     </row>
     <row r="129" ht="14.25" customHeight="1">
       <c r="A129" s="48"/>
-      <c r="B129" s="49"/>
-      <c r="C129" s="50"/>
-      <c r="D129" s="51"/>
+      <c r="B129" s="50"/>
+      <c r="C129" s="51"/>
+      <c r="D129" s="52"/>
       <c r="E129" s="25"/>
       <c r="F129" s="23"/>
       <c r="G129" s="27"/>
@@ -7172,7 +7297,7 @@
       <c r="Z129" s="20"/>
     </row>
     <row r="130" ht="14.25" customHeight="1">
-      <c r="A130" s="52"/>
+      <c r="A130" s="49"/>
       <c r="B130" s="53"/>
       <c r="C130" s="54"/>
       <c r="D130" s="55"/>
@@ -7201,9 +7326,9 @@
     </row>
     <row r="131" ht="14.25" customHeight="1">
       <c r="A131" s="48"/>
-      <c r="B131" s="49"/>
-      <c r="C131" s="50"/>
-      <c r="D131" s="51"/>
+      <c r="B131" s="50"/>
+      <c r="C131" s="51"/>
+      <c r="D131" s="52"/>
       <c r="E131" s="25"/>
       <c r="F131" s="23"/>
       <c r="G131" s="27"/>
@@ -7228,7 +7353,7 @@
       <c r="Z131" s="20"/>
     </row>
     <row r="132" ht="14.25" customHeight="1">
-      <c r="A132" s="52"/>
+      <c r="A132" s="49"/>
       <c r="B132" s="53"/>
       <c r="C132" s="54"/>
       <c r="D132" s="55"/>
@@ -7257,9 +7382,9 @@
     </row>
     <row r="133" ht="14.25" customHeight="1">
       <c r="A133" s="48"/>
-      <c r="B133" s="49"/>
-      <c r="C133" s="50"/>
-      <c r="D133" s="51"/>
+      <c r="B133" s="50"/>
+      <c r="C133" s="51"/>
+      <c r="D133" s="52"/>
       <c r="E133" s="25"/>
       <c r="F133" s="23"/>
       <c r="G133" s="27"/>
@@ -7284,7 +7409,7 @@
       <c r="Z133" s="20"/>
     </row>
     <row r="134" ht="14.25" customHeight="1">
-      <c r="A134" s="52"/>
+      <c r="A134" s="49"/>
       <c r="B134" s="53"/>
       <c r="C134" s="54"/>
       <c r="D134" s="55"/>
@@ -7313,9 +7438,9 @@
     </row>
     <row r="135" ht="14.25" customHeight="1">
       <c r="A135" s="48"/>
-      <c r="B135" s="49"/>
-      <c r="C135" s="50"/>
-      <c r="D135" s="51"/>
+      <c r="B135" s="50"/>
+      <c r="C135" s="51"/>
+      <c r="D135" s="52"/>
       <c r="E135" s="25"/>
       <c r="F135" s="23"/>
       <c r="G135" s="27"/>
@@ -7340,7 +7465,7 @@
       <c r="Z135" s="20"/>
     </row>
     <row r="136" ht="14.25" customHeight="1">
-      <c r="A136" s="52"/>
+      <c r="A136" s="49"/>
       <c r="B136" s="53"/>
       <c r="C136" s="54"/>
       <c r="D136" s="55"/>
@@ -7369,9 +7494,9 @@
     </row>
     <row r="137" ht="14.25" customHeight="1">
       <c r="A137" s="48"/>
-      <c r="B137" s="49"/>
-      <c r="C137" s="50"/>
-      <c r="D137" s="51"/>
+      <c r="B137" s="50"/>
+      <c r="C137" s="51"/>
+      <c r="D137" s="52"/>
       <c r="E137" s="25"/>
       <c r="F137" s="23"/>
       <c r="G137" s="27"/>
@@ -7396,7 +7521,7 @@
       <c r="Z137" s="20"/>
     </row>
     <row r="138" ht="14.25" customHeight="1">
-      <c r="A138" s="52"/>
+      <c r="A138" s="49"/>
       <c r="B138" s="53"/>
       <c r="C138" s="54"/>
       <c r="D138" s="55"/>
@@ -7425,9 +7550,9 @@
     </row>
     <row r="139" ht="14.25" customHeight="1">
       <c r="A139" s="48"/>
-      <c r="B139" s="49"/>
-      <c r="C139" s="50"/>
-      <c r="D139" s="51"/>
+      <c r="B139" s="50"/>
+      <c r="C139" s="51"/>
+      <c r="D139" s="52"/>
       <c r="E139" s="25"/>
       <c r="F139" s="23"/>
       <c r="G139" s="27"/>
@@ -7452,7 +7577,7 @@
       <c r="Z139" s="20"/>
     </row>
     <row r="140" ht="14.25" customHeight="1">
-      <c r="A140" s="52"/>
+      <c r="A140" s="49"/>
       <c r="B140" s="53"/>
       <c r="C140" s="54"/>
       <c r="D140" s="55"/>
@@ -7481,9 +7606,9 @@
     </row>
     <row r="141" ht="14.25" customHeight="1">
       <c r="A141" s="48"/>
-      <c r="B141" s="49"/>
-      <c r="C141" s="50"/>
-      <c r="D141" s="51"/>
+      <c r="B141" s="50"/>
+      <c r="C141" s="51"/>
+      <c r="D141" s="52"/>
       <c r="E141" s="25"/>
       <c r="F141" s="23"/>
       <c r="G141" s="27"/>
@@ -7508,7 +7633,7 @@
       <c r="Z141" s="20"/>
     </row>
     <row r="142" ht="14.25" customHeight="1">
-      <c r="A142" s="52"/>
+      <c r="A142" s="49"/>
       <c r="B142" s="53"/>
       <c r="C142" s="54"/>
       <c r="D142" s="55"/>
@@ -7537,9 +7662,9 @@
     </row>
     <row r="143" ht="14.25" customHeight="1">
       <c r="A143" s="48"/>
-      <c r="B143" s="49"/>
-      <c r="C143" s="50"/>
-      <c r="D143" s="51"/>
+      <c r="B143" s="50"/>
+      <c r="C143" s="51"/>
+      <c r="D143" s="52"/>
       <c r="E143" s="25"/>
       <c r="F143" s="23"/>
       <c r="G143" s="27"/>
@@ -7564,7 +7689,7 @@
       <c r="Z143" s="20"/>
     </row>
     <row r="144" ht="14.25" customHeight="1">
-      <c r="A144" s="52"/>
+      <c r="A144" s="49"/>
       <c r="B144" s="53"/>
       <c r="C144" s="54"/>
       <c r="D144" s="55"/>
@@ -7593,9 +7718,9 @@
     </row>
     <row r="145" ht="14.25" customHeight="1">
       <c r="A145" s="48"/>
-      <c r="B145" s="49"/>
-      <c r="C145" s="50"/>
-      <c r="D145" s="51"/>
+      <c r="B145" s="50"/>
+      <c r="C145" s="51"/>
+      <c r="D145" s="52"/>
       <c r="E145" s="25"/>
       <c r="F145" s="23"/>
       <c r="G145" s="27"/>
@@ -7620,7 +7745,7 @@
       <c r="Z145" s="20"/>
     </row>
     <row r="146" ht="14.25" customHeight="1">
-      <c r="A146" s="52"/>
+      <c r="A146" s="49"/>
       <c r="B146" s="53"/>
       <c r="C146" s="54"/>
       <c r="D146" s="55"/>
@@ -7649,9 +7774,9 @@
     </row>
     <row r="147" ht="14.25" customHeight="1">
       <c r="A147" s="48"/>
-      <c r="B147" s="49"/>
-      <c r="C147" s="50"/>
-      <c r="D147" s="51"/>
+      <c r="B147" s="50"/>
+      <c r="C147" s="51"/>
+      <c r="D147" s="52"/>
       <c r="E147" s="25"/>
       <c r="F147" s="23"/>
       <c r="G147" s="27"/>
@@ -7676,7 +7801,7 @@
       <c r="Z147" s="20"/>
     </row>
     <row r="148" ht="14.25" customHeight="1">
-      <c r="A148" s="52"/>
+      <c r="A148" s="49"/>
       <c r="B148" s="53"/>
       <c r="C148" s="54"/>
       <c r="D148" s="55"/>
@@ -7705,9 +7830,9 @@
     </row>
     <row r="149" ht="14.25" customHeight="1">
       <c r="A149" s="48"/>
-      <c r="B149" s="49"/>
-      <c r="C149" s="50"/>
-      <c r="D149" s="51"/>
+      <c r="B149" s="50"/>
+      <c r="C149" s="51"/>
+      <c r="D149" s="52"/>
       <c r="E149" s="25"/>
       <c r="F149" s="23"/>
       <c r="G149" s="27"/>
@@ -7732,7 +7857,7 @@
       <c r="Z149" s="20"/>
     </row>
     <row r="150" ht="14.25" customHeight="1">
-      <c r="A150" s="52"/>
+      <c r="A150" s="49"/>
       <c r="B150" s="53"/>
       <c r="C150" s="54"/>
       <c r="D150" s="55"/>
@@ -7761,9 +7886,9 @@
     </row>
     <row r="151" ht="14.25" customHeight="1">
       <c r="A151" s="48"/>
-      <c r="B151" s="49"/>
-      <c r="C151" s="50"/>
-      <c r="D151" s="51"/>
+      <c r="B151" s="50"/>
+      <c r="C151" s="51"/>
+      <c r="D151" s="52"/>
       <c r="E151" s="25"/>
       <c r="F151" s="23"/>
       <c r="G151" s="27"/>
@@ -7788,7 +7913,7 @@
       <c r="Z151" s="20"/>
     </row>
     <row r="152" ht="14.25" customHeight="1">
-      <c r="A152" s="52"/>
+      <c r="A152" s="49"/>
       <c r="B152" s="53"/>
       <c r="C152" s="54"/>
       <c r="D152" s="55"/>
@@ -7817,9 +7942,9 @@
     </row>
     <row r="153" ht="14.25" customHeight="1">
       <c r="A153" s="48"/>
-      <c r="B153" s="49"/>
-      <c r="C153" s="50"/>
-      <c r="D153" s="51"/>
+      <c r="B153" s="50"/>
+      <c r="C153" s="51"/>
+      <c r="D153" s="52"/>
       <c r="E153" s="25"/>
       <c r="F153" s="23"/>
       <c r="G153" s="27"/>
@@ -7844,7 +7969,7 @@
       <c r="Z153" s="20"/>
     </row>
     <row r="154" ht="14.25" customHeight="1">
-      <c r="A154" s="52"/>
+      <c r="A154" s="49"/>
       <c r="B154" s="53"/>
       <c r="C154" s="54"/>
       <c r="D154" s="55"/>
@@ -7873,9 +7998,9 @@
     </row>
     <row r="155" ht="14.25" customHeight="1">
       <c r="A155" s="48"/>
-      <c r="B155" s="49"/>
-      <c r="C155" s="50"/>
-      <c r="D155" s="51"/>
+      <c r="B155" s="50"/>
+      <c r="C155" s="51"/>
+      <c r="D155" s="52"/>
       <c r="E155" s="25"/>
       <c r="F155" s="23"/>
       <c r="G155" s="27"/>
@@ -7900,7 +8025,7 @@
       <c r="Z155" s="20"/>
     </row>
     <row r="156" ht="14.25" customHeight="1">
-      <c r="A156" s="52"/>
+      <c r="A156" s="49"/>
       <c r="B156" s="53"/>
       <c r="C156" s="54"/>
       <c r="D156" s="55"/>
@@ -7929,9 +8054,9 @@
     </row>
     <row r="157" ht="14.25" customHeight="1">
       <c r="A157" s="48"/>
-      <c r="B157" s="49"/>
-      <c r="C157" s="50"/>
-      <c r="D157" s="51"/>
+      <c r="B157" s="50"/>
+      <c r="C157" s="51"/>
+      <c r="D157" s="52"/>
       <c r="E157" s="25"/>
       <c r="F157" s="23"/>
       <c r="G157" s="27"/>
@@ -7956,7 +8081,7 @@
       <c r="Z157" s="20"/>
     </row>
     <row r="158" ht="14.25" customHeight="1">
-      <c r="A158" s="52"/>
+      <c r="A158" s="49"/>
       <c r="B158" s="53"/>
       <c r="C158" s="54"/>
       <c r="D158" s="55"/>
@@ -7985,9 +8110,9 @@
     </row>
     <row r="159" ht="14.25" customHeight="1">
       <c r="A159" s="48"/>
-      <c r="B159" s="49"/>
-      <c r="C159" s="50"/>
-      <c r="D159" s="51"/>
+      <c r="B159" s="50"/>
+      <c r="C159" s="51"/>
+      <c r="D159" s="52"/>
       <c r="E159" s="25"/>
       <c r="F159" s="23"/>
       <c r="G159" s="27"/>
@@ -8012,7 +8137,7 @@
       <c r="Z159" s="20"/>
     </row>
     <row r="160" ht="14.25" customHeight="1">
-      <c r="A160" s="52"/>
+      <c r="A160" s="49"/>
       <c r="B160" s="53"/>
       <c r="C160" s="54"/>
       <c r="D160" s="55"/>
@@ -8041,9 +8166,9 @@
     </row>
     <row r="161" ht="14.25" customHeight="1">
       <c r="A161" s="48"/>
-      <c r="B161" s="49"/>
-      <c r="C161" s="50"/>
-      <c r="D161" s="51"/>
+      <c r="B161" s="50"/>
+      <c r="C161" s="51"/>
+      <c r="D161" s="52"/>
       <c r="E161" s="25"/>
       <c r="F161" s="23"/>
       <c r="G161" s="27"/>
@@ -8068,7 +8193,7 @@
       <c r="Z161" s="20"/>
     </row>
     <row r="162" ht="14.25" customHeight="1">
-      <c r="A162" s="52"/>
+      <c r="A162" s="49"/>
       <c r="B162" s="53"/>
       <c r="C162" s="54"/>
       <c r="D162" s="55"/>
@@ -8097,9 +8222,9 @@
     </row>
     <row r="163" ht="14.25" customHeight="1">
       <c r="A163" s="48"/>
-      <c r="B163" s="49"/>
-      <c r="C163" s="50"/>
-      <c r="D163" s="51"/>
+      <c r="B163" s="50"/>
+      <c r="C163" s="51"/>
+      <c r="D163" s="52"/>
       <c r="E163" s="25"/>
       <c r="F163" s="23"/>
       <c r="G163" s="27"/>
@@ -8124,7 +8249,7 @@
       <c r="Z163" s="20"/>
     </row>
     <row r="164" ht="14.25" customHeight="1">
-      <c r="A164" s="52"/>
+      <c r="A164" s="49"/>
       <c r="B164" s="53"/>
       <c r="C164" s="54"/>
       <c r="D164" s="55"/>
@@ -8153,9 +8278,9 @@
     </row>
     <row r="165" ht="14.25" customHeight="1">
       <c r="A165" s="48"/>
-      <c r="B165" s="49"/>
-      <c r="C165" s="50"/>
-      <c r="D165" s="51"/>
+      <c r="B165" s="50"/>
+      <c r="C165" s="51"/>
+      <c r="D165" s="52"/>
       <c r="E165" s="25"/>
       <c r="F165" s="23"/>
       <c r="G165" s="27"/>
@@ -8180,7 +8305,7 @@
       <c r="Z165" s="20"/>
     </row>
     <row r="166" ht="14.25" customHeight="1">
-      <c r="A166" s="52"/>
+      <c r="A166" s="49"/>
       <c r="B166" s="53"/>
       <c r="C166" s="54"/>
       <c r="D166" s="55"/>
@@ -8209,9 +8334,9 @@
     </row>
     <row r="167" ht="14.25" customHeight="1">
       <c r="A167" s="48"/>
-      <c r="B167" s="49"/>
-      <c r="C167" s="50"/>
-      <c r="D167" s="51"/>
+      <c r="B167" s="50"/>
+      <c r="C167" s="51"/>
+      <c r="D167" s="52"/>
       <c r="E167" s="25"/>
       <c r="F167" s="23"/>
       <c r="G167" s="27"/>
@@ -8236,7 +8361,7 @@
       <c r="Z167" s="20"/>
     </row>
     <row r="168" ht="14.25" customHeight="1">
-      <c r="A168" s="52"/>
+      <c r="A168" s="49"/>
       <c r="B168" s="53"/>
       <c r="C168" s="54"/>
       <c r="D168" s="55"/>
@@ -8265,9 +8390,9 @@
     </row>
     <row r="169" ht="14.25" customHeight="1">
       <c r="A169" s="48"/>
-      <c r="B169" s="49"/>
-      <c r="C169" s="50"/>
-      <c r="D169" s="51"/>
+      <c r="B169" s="50"/>
+      <c r="C169" s="51"/>
+      <c r="D169" s="52"/>
       <c r="E169" s="25"/>
       <c r="F169" s="23"/>
       <c r="G169" s="27"/>
@@ -8292,7 +8417,7 @@
       <c r="Z169" s="20"/>
     </row>
     <row r="170" ht="14.25" customHeight="1">
-      <c r="A170" s="52"/>
+      <c r="A170" s="49"/>
       <c r="B170" s="53"/>
       <c r="C170" s="54"/>
       <c r="D170" s="55"/>
@@ -8321,9 +8446,9 @@
     </row>
     <row r="171" ht="14.25" customHeight="1">
       <c r="A171" s="48"/>
-      <c r="B171" s="49"/>
-      <c r="C171" s="50"/>
-      <c r="D171" s="51"/>
+      <c r="B171" s="50"/>
+      <c r="C171" s="51"/>
+      <c r="D171" s="52"/>
       <c r="E171" s="25"/>
       <c r="F171" s="23"/>
       <c r="G171" s="27"/>
@@ -8348,7 +8473,7 @@
       <c r="Z171" s="20"/>
     </row>
     <row r="172" ht="14.25" customHeight="1">
-      <c r="A172" s="52"/>
+      <c r="A172" s="49"/>
       <c r="B172" s="53"/>
       <c r="C172" s="54"/>
       <c r="D172" s="55"/>
@@ -8377,9 +8502,9 @@
     </row>
     <row r="173" ht="14.25" customHeight="1">
       <c r="A173" s="48"/>
-      <c r="B173" s="49"/>
-      <c r="C173" s="50"/>
-      <c r="D173" s="51"/>
+      <c r="B173" s="50"/>
+      <c r="C173" s="51"/>
+      <c r="D173" s="52"/>
       <c r="E173" s="25"/>
       <c r="F173" s="23"/>
       <c r="G173" s="27"/>
@@ -8404,7 +8529,7 @@
       <c r="Z173" s="20"/>
     </row>
     <row r="174" ht="14.25" customHeight="1">
-      <c r="A174" s="52"/>
+      <c r="A174" s="49"/>
       <c r="B174" s="53"/>
       <c r="C174" s="54"/>
       <c r="D174" s="55"/>
@@ -8433,9 +8558,9 @@
     </row>
     <row r="175" ht="14.25" customHeight="1">
       <c r="A175" s="48"/>
-      <c r="B175" s="49"/>
-      <c r="C175" s="50"/>
-      <c r="D175" s="51"/>
+      <c r="B175" s="50"/>
+      <c r="C175" s="51"/>
+      <c r="D175" s="52"/>
       <c r="E175" s="25"/>
       <c r="F175" s="23"/>
       <c r="G175" s="27"/>
@@ -8460,7 +8585,7 @@
       <c r="Z175" s="20"/>
     </row>
     <row r="176" ht="14.25" customHeight="1">
-      <c r="A176" s="52"/>
+      <c r="A176" s="49"/>
       <c r="B176" s="53"/>
       <c r="C176" s="54"/>
       <c r="D176" s="55"/>
@@ -8489,9 +8614,9 @@
     </row>
     <row r="177" ht="14.25" customHeight="1">
       <c r="A177" s="48"/>
-      <c r="B177" s="49"/>
-      <c r="C177" s="50"/>
-      <c r="D177" s="51"/>
+      <c r="B177" s="50"/>
+      <c r="C177" s="51"/>
+      <c r="D177" s="52"/>
       <c r="E177" s="25"/>
       <c r="F177" s="23"/>
       <c r="G177" s="27"/>
@@ -8516,7 +8641,7 @@
       <c r="Z177" s="20"/>
     </row>
     <row r="178" ht="14.25" customHeight="1">
-      <c r="A178" s="52"/>
+      <c r="A178" s="49"/>
       <c r="B178" s="53"/>
       <c r="C178" s="54"/>
       <c r="D178" s="55"/>
@@ -8545,9 +8670,9 @@
     </row>
     <row r="179" ht="14.25" customHeight="1">
       <c r="A179" s="48"/>
-      <c r="B179" s="49"/>
-      <c r="C179" s="50"/>
-      <c r="D179" s="51"/>
+      <c r="B179" s="50"/>
+      <c r="C179" s="51"/>
+      <c r="D179" s="52"/>
       <c r="E179" s="25"/>
       <c r="F179" s="23"/>
       <c r="G179" s="27"/>
@@ -8572,7 +8697,7 @@
       <c r="Z179" s="20"/>
     </row>
     <row r="180" ht="14.25" customHeight="1">
-      <c r="A180" s="52"/>
+      <c r="A180" s="49"/>
       <c r="B180" s="53"/>
       <c r="C180" s="54"/>
       <c r="D180" s="55"/>
@@ -8601,9 +8726,9 @@
     </row>
     <row r="181" ht="14.25" customHeight="1">
       <c r="A181" s="48"/>
-      <c r="B181" s="49"/>
-      <c r="C181" s="50"/>
-      <c r="D181" s="51"/>
+      <c r="B181" s="50"/>
+      <c r="C181" s="51"/>
+      <c r="D181" s="52"/>
       <c r="E181" s="25"/>
       <c r="F181" s="23"/>
       <c r="G181" s="27"/>
@@ -8628,7 +8753,7 @@
       <c r="Z181" s="20"/>
     </row>
     <row r="182" ht="14.25" customHeight="1">
-      <c r="A182" s="52"/>
+      <c r="A182" s="49"/>
       <c r="B182" s="53"/>
       <c r="C182" s="54"/>
       <c r="D182" s="55"/>
@@ -8657,9 +8782,9 @@
     </row>
     <row r="183" ht="14.25" customHeight="1">
       <c r="A183" s="48"/>
-      <c r="B183" s="49"/>
-      <c r="C183" s="50"/>
-      <c r="D183" s="51"/>
+      <c r="B183" s="50"/>
+      <c r="C183" s="51"/>
+      <c r="D183" s="52"/>
       <c r="E183" s="25"/>
       <c r="F183" s="23"/>
       <c r="G183" s="27"/>
@@ -8684,7 +8809,7 @@
       <c r="Z183" s="20"/>
     </row>
     <row r="184" ht="14.25" customHeight="1">
-      <c r="A184" s="52"/>
+      <c r="A184" s="49"/>
       <c r="B184" s="53"/>
       <c r="C184" s="54"/>
       <c r="D184" s="55"/>
@@ -8713,9 +8838,9 @@
     </row>
     <row r="185" ht="14.25" customHeight="1">
       <c r="A185" s="48"/>
-      <c r="B185" s="49"/>
-      <c r="C185" s="50"/>
-      <c r="D185" s="51"/>
+      <c r="B185" s="50"/>
+      <c r="C185" s="51"/>
+      <c r="D185" s="52"/>
       <c r="E185" s="25"/>
       <c r="F185" s="23"/>
       <c r="G185" s="27"/>
@@ -8740,7 +8865,7 @@
       <c r="Z185" s="20"/>
     </row>
     <row r="186" ht="14.25" customHeight="1">
-      <c r="A186" s="52"/>
+      <c r="A186" s="49"/>
       <c r="B186" s="53"/>
       <c r="C186" s="54"/>
       <c r="D186" s="55"/>
@@ -8769,9 +8894,9 @@
     </row>
     <row r="187" ht="14.25" customHeight="1">
       <c r="A187" s="48"/>
-      <c r="B187" s="49"/>
-      <c r="C187" s="50"/>
-      <c r="D187" s="51"/>
+      <c r="B187" s="50"/>
+      <c r="C187" s="51"/>
+      <c r="D187" s="52"/>
       <c r="E187" s="25"/>
       <c r="F187" s="23"/>
       <c r="G187" s="27"/>
@@ -8796,7 +8921,7 @@
       <c r="Z187" s="20"/>
     </row>
     <row r="188" ht="14.25" customHeight="1">
-      <c r="A188" s="52"/>
+      <c r="A188" s="49"/>
       <c r="B188" s="53"/>
       <c r="C188" s="54"/>
       <c r="D188" s="55"/>
@@ -8825,9 +8950,9 @@
     </row>
     <row r="189" ht="14.25" customHeight="1">
       <c r="A189" s="48"/>
-      <c r="B189" s="49"/>
-      <c r="C189" s="50"/>
-      <c r="D189" s="51"/>
+      <c r="B189" s="50"/>
+      <c r="C189" s="51"/>
+      <c r="D189" s="52"/>
       <c r="E189" s="25"/>
       <c r="F189" s="23"/>
       <c r="G189" s="27"/>
@@ -8852,7 +8977,7 @@
       <c r="Z189" s="20"/>
     </row>
     <row r="190" ht="14.25" customHeight="1">
-      <c r="A190" s="52"/>
+      <c r="A190" s="49"/>
       <c r="B190" s="53"/>
       <c r="C190" s="54"/>
       <c r="D190" s="55"/>
@@ -8881,9 +9006,9 @@
     </row>
     <row r="191" ht="14.25" customHeight="1">
       <c r="A191" s="48"/>
-      <c r="B191" s="49"/>
-      <c r="C191" s="50"/>
-      <c r="D191" s="51"/>
+      <c r="B191" s="50"/>
+      <c r="C191" s="51"/>
+      <c r="D191" s="52"/>
       <c r="E191" s="25"/>
       <c r="F191" s="23"/>
       <c r="G191" s="27"/>
@@ -8908,7 +9033,7 @@
       <c r="Z191" s="20"/>
     </row>
     <row r="192" ht="14.25" customHeight="1">
-      <c r="A192" s="52"/>
+      <c r="A192" s="49"/>
       <c r="B192" s="53"/>
       <c r="C192" s="54"/>
       <c r="D192" s="55"/>
@@ -8937,9 +9062,9 @@
     </row>
     <row r="193" ht="14.25" customHeight="1">
       <c r="A193" s="48"/>
-      <c r="B193" s="49"/>
-      <c r="C193" s="50"/>
-      <c r="D193" s="51"/>
+      <c r="B193" s="50"/>
+      <c r="C193" s="51"/>
+      <c r="D193" s="52"/>
       <c r="E193" s="25"/>
       <c r="F193" s="23"/>
       <c r="G193" s="27"/>
@@ -8964,7 +9089,7 @@
       <c r="Z193" s="20"/>
     </row>
     <row r="194" ht="14.25" customHeight="1">
-      <c r="A194" s="52"/>
+      <c r="A194" s="49"/>
       <c r="B194" s="53"/>
       <c r="C194" s="54"/>
       <c r="D194" s="55"/>
@@ -8993,9 +9118,9 @@
     </row>
     <row r="195" ht="14.25" customHeight="1">
       <c r="A195" s="48"/>
-      <c r="B195" s="49"/>
-      <c r="C195" s="50"/>
-      <c r="D195" s="51"/>
+      <c r="B195" s="50"/>
+      <c r="C195" s="51"/>
+      <c r="D195" s="52"/>
       <c r="E195" s="25"/>
       <c r="F195" s="23"/>
       <c r="G195" s="27"/>
@@ -9020,7 +9145,7 @@
       <c r="Z195" s="20"/>
     </row>
     <row r="196" ht="14.25" customHeight="1">
-      <c r="A196" s="52"/>
+      <c r="A196" s="49"/>
       <c r="B196" s="53"/>
       <c r="C196" s="54"/>
       <c r="D196" s="55"/>
@@ -9049,9 +9174,9 @@
     </row>
     <row r="197" ht="14.25" customHeight="1">
       <c r="A197" s="48"/>
-      <c r="B197" s="49"/>
-      <c r="C197" s="50"/>
-      <c r="D197" s="51"/>
+      <c r="B197" s="50"/>
+      <c r="C197" s="51"/>
+      <c r="D197" s="52"/>
       <c r="E197" s="25"/>
       <c r="F197" s="23"/>
       <c r="G197" s="27"/>
@@ -9076,7 +9201,7 @@
       <c r="Z197" s="20"/>
     </row>
     <row r="198" ht="14.25" customHeight="1">
-      <c r="A198" s="52"/>
+      <c r="A198" s="49"/>
       <c r="B198" s="53"/>
       <c r="C198" s="54"/>
       <c r="D198" s="55"/>
@@ -9105,9 +9230,9 @@
     </row>
     <row r="199" ht="14.25" customHeight="1">
       <c r="A199" s="48"/>
-      <c r="B199" s="49"/>
-      <c r="C199" s="50"/>
-      <c r="D199" s="51"/>
+      <c r="B199" s="50"/>
+      <c r="C199" s="51"/>
+      <c r="D199" s="52"/>
       <c r="E199" s="25"/>
       <c r="F199" s="23"/>
       <c r="G199" s="27"/>
@@ -31614,13 +31739,16 @@
     <hyperlink r:id="rId40" ref="A72"/>
     <hyperlink r:id="rId41" ref="A73"/>
     <hyperlink r:id="rId42" ref="A74"/>
+    <hyperlink r:id="rId43" ref="A76"/>
+    <hyperlink r:id="rId44" ref="A77"/>
+    <hyperlink r:id="rId45" ref="K77"/>
   </hyperlinks>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId43"/>
+  <drawing r:id="rId46"/>
   <tableParts count="1">
-    <tablePart r:id="rId45"/>
+    <tablePart r:id="rId48"/>
   </tableParts>
 </worksheet>
 </file>
@@ -31642,10 +31770,10 @@
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
       <c r="A1" s="68" t="s">
-        <v>348</v>
+        <v>356</v>
       </c>
       <c r="B1" s="68" t="s">
-        <v>349</v>
+        <v>357</v>
       </c>
       <c r="C1" s="68"/>
       <c r="D1" s="68"/>
@@ -31677,7 +31805,7 @@
         <v>13</v>
       </c>
       <c r="B2" s="70" t="s">
-        <v>350</v>
+        <v>358</v>
       </c>
     </row>
     <row r="3" ht="14.25" customHeight="1">
@@ -31685,7 +31813,7 @@
         <v>32</v>
       </c>
       <c r="B3" s="70" t="s">
-        <v>351</v>
+        <v>359</v>
       </c>
     </row>
     <row r="4" ht="14.25" customHeight="1">
@@ -31693,7 +31821,7 @@
         <v>46</v>
       </c>
       <c r="B4" s="70" t="s">
-        <v>352</v>
+        <v>360</v>
       </c>
     </row>
     <row r="5" ht="14.25" customHeight="1">
@@ -31701,7 +31829,7 @@
         <v>21</v>
       </c>
       <c r="B5" s="70" t="s">
-        <v>353</v>
+        <v>361</v>
       </c>
     </row>
     <row r="6" ht="14.25" customHeight="1">
@@ -31709,7 +31837,7 @@
         <v>59</v>
       </c>
       <c r="B6" s="70" t="s">
-        <v>354</v>
+        <v>362</v>
       </c>
     </row>
     <row r="7" ht="14.25" customHeight="1">
@@ -31717,7 +31845,7 @@
         <v>154</v>
       </c>
       <c r="B7" s="70" t="s">
-        <v>355</v>
+        <v>363</v>
       </c>
     </row>
     <row r="8" ht="14.25" customHeight="1">

</xml_diff>